<commit_message>
additional work on results and findings doc
</commit_message>
<xml_diff>
--- a/Data/bih_municipality_reorg_crosswalk.xlsx
+++ b/Data/bih_municipality_reorg_crosswalk.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmyballesteros/R/bih_voting/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B47E54E-7348-A54B-A63F-BEB66B273DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338E380F-7E51-AE4B-9F9F-F609E9D33257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7680" yWindow="760" windowWidth="26880" windowHeight="20880" xr2:uid="{13B4E9CA-A51D-8D4A-83FE-B4D16F794EC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="156">
   <si>
     <t>Trebinje</t>
   </si>
@@ -501,13 +501,16 @@
   </si>
   <si>
     <t>Sarajevo Vogošća</t>
+  </si>
+  <si>
+    <t>Modified</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -522,13 +525,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
@@ -555,11 +551,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,7 +898,7 @@
   <dimension ref="A1:F143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -914,6 +915,9 @@
       <c r="B1" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -922,6 +926,10 @@
       <c r="B2" s="2" t="s">
         <v>117</v>
       </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -930,7 +938,10 @@
       <c r="B3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -939,7 +950,9 @@
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -948,7 +961,10 @@
       <c r="B5" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -957,7 +973,10 @@
       <c r="B6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -966,7 +985,10 @@
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -975,7 +997,11 @@
       <c r="B8" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -984,8 +1010,11 @@
       <c r="B9" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -994,7 +1023,10 @@
       <c r="B10" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -1003,7 +1035,11 @@
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -1012,7 +1048,10 @@
       <c r="B12" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -1021,7 +1060,10 @@
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -1030,7 +1072,10 @@
       <c r="B14" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -1039,7 +1084,10 @@
       <c r="B15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -1048,295 +1096,389 @@
       <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E36" s="3"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C40" s="1">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C42" s="1">
+        <v>1</v>
+      </c>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E43" s="3"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E46" s="3"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E47" s="3"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E48" s="3"/>
+      <c r="C48" s="1">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
@@ -1345,8 +1487,10 @@
       <c r="B49" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E49" s="3"/>
-      <c r="F49" s="2"/>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
@@ -1355,7 +1499,9 @@
       <c r="B50" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E50" s="3"/>
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
@@ -1364,7 +1510,10 @@
       <c r="B51" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E51" s="3"/>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51" s="3"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
@@ -1373,7 +1522,9 @@
       <c r="B52" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E52" s="3"/>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
@@ -1382,7 +1533,9 @@
       <c r="B53" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E53" s="3"/>
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
@@ -1391,7 +1544,9 @@
       <c r="B54" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E54" s="3"/>
+      <c r="C54" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
@@ -1400,7 +1555,10 @@
       <c r="B55" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E55" s="3"/>
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+      <c r="F55" s="3"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
@@ -1409,7 +1567,10 @@
       <c r="B56" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E56" s="3"/>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="F56" s="3"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
@@ -1418,7 +1579,9 @@
       <c r="B57" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E57" s="3"/>
+      <c r="C57" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
@@ -1427,7 +1590,9 @@
       <c r="B58" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E58" s="3"/>
+      <c r="C58" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
@@ -1436,7 +1601,10 @@
       <c r="B59" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E59" s="3"/>
+      <c r="C59" s="1">
+        <v>0</v>
+      </c>
+      <c r="F59" s="3"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
@@ -1445,7 +1613,9 @@
       <c r="B60" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E60" s="3"/>
+      <c r="C60" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
@@ -1454,7 +1624,10 @@
       <c r="B61" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E61" s="3"/>
+      <c r="C61" s="1">
+        <v>0</v>
+      </c>
+      <c r="F61" s="3"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
@@ -1463,7 +1636,10 @@
       <c r="B62" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E62" s="3"/>
+      <c r="C62" s="1">
+        <v>1</v>
+      </c>
+      <c r="F62" s="3"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
@@ -1472,7 +1648,10 @@
       <c r="B63" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E63" s="3"/>
+      <c r="C63" s="1">
+        <v>0</v>
+      </c>
+      <c r="F63" s="3"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
@@ -1481,685 +1660,937 @@
       <c r="B64" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E64" s="3"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E65" s="3"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C65" s="1">
+        <v>0</v>
+      </c>
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E66" s="3"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C66" s="1">
+        <v>0</v>
+      </c>
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E67" s="3"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C67" s="1">
+        <v>1</v>
+      </c>
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E68" s="3"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C68" s="1">
+        <v>1</v>
+      </c>
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E69" s="3"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C69" s="1">
+        <v>1</v>
+      </c>
+      <c r="E69" s="2"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E70" s="3"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C70" s="1">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E71" s="3"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C71" s="1">
+        <v>0</v>
+      </c>
+      <c r="F71" s="3"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E72" s="3"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C72" s="1">
+        <v>0</v>
+      </c>
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E73" s="3"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C73" s="1">
+        <v>0</v>
+      </c>
+      <c r="F73" s="3"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E74" s="3"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C74" s="1">
+        <v>1</v>
+      </c>
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E75" s="3"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C75" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E76" s="3"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C76" s="1">
+        <v>0</v>
+      </c>
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E77" s="3"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C77" s="1">
+        <v>1</v>
+      </c>
+      <c r="F77" s="4"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E78" s="3"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C78" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E79" s="3"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C79" s="1">
+        <v>1</v>
+      </c>
+      <c r="F79" s="3"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E80" s="3"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C80" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E81" s="3"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C81" s="1">
+        <v>0</v>
+      </c>
+      <c r="F81" s="3"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E82" s="3"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C82" s="1">
+        <v>0</v>
+      </c>
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E83" s="3"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C83" s="1">
+        <v>1</v>
+      </c>
+      <c r="F83" s="3"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E84" s="3"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C84" s="1">
+        <v>0</v>
+      </c>
+      <c r="E84" s="2"/>
+      <c r="F84" s="3"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E85" s="3"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C85" s="1">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2"/>
+      <c r="F85" s="3"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E86" s="3"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C86" s="1">
+        <v>1</v>
+      </c>
+      <c r="F86" s="3"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E87" s="3"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C87" s="1">
+        <v>1</v>
+      </c>
+      <c r="E87" s="2"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E88" s="3"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C88" s="1">
+        <v>0</v>
+      </c>
+      <c r="F88" s="3"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E89" s="3"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C89" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E90" s="3"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C90" s="1">
+        <v>1</v>
+      </c>
+      <c r="F90" s="3"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E91" s="3"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C91" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E92" s="3"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C92" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E93" s="3"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C93" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E94" s="3"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C94" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E95" s="3"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C95" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E96" s="3"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C96" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E97" s="3"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C97" s="1">
+        <v>0</v>
+      </c>
+      <c r="F97" s="3"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E98" s="3"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C98" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E99" s="3"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C99" s="1">
+        <v>0</v>
+      </c>
+      <c r="F99" s="3"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E100" s="3"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C100" s="1">
+        <v>0</v>
+      </c>
+      <c r="F100" s="3"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E101" s="3"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C101" s="1">
+        <v>1</v>
+      </c>
+      <c r="F101" s="3"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E102" s="3"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C102" s="1">
+        <v>1</v>
+      </c>
+      <c r="F102" s="3"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E103" s="3"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C103" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E104" s="3"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C104" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E105" s="3"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C105" s="1">
+        <v>1</v>
+      </c>
+      <c r="F105" s="3"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E106" s="3"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C106" s="1">
+        <v>1</v>
+      </c>
+      <c r="F106" s="3"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E107" s="3"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C107" s="1">
+        <v>1</v>
+      </c>
+      <c r="F107" s="3"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E108" s="3"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C108" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E109" s="3"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C109" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E110" s="3"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C110" s="1">
+        <v>1</v>
+      </c>
+      <c r="F110" s="3"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E111" s="3"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C111" s="1">
+        <v>0</v>
+      </c>
+      <c r="F111" s="3"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C112" s="1">
+        <v>0</v>
+      </c>
+      <c r="F112" s="3"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>146</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C113" s="1">
+        <v>0</v>
+      </c>
+      <c r="E113" s="2"/>
+      <c r="F113" s="3"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>144</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C114" s="1">
+        <v>1</v>
+      </c>
+      <c r="F114" s="3"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C115" s="1">
+        <v>0</v>
+      </c>
+      <c r="F115" s="3"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C116" s="1">
+        <v>0</v>
+      </c>
+      <c r="F116" s="3"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C117" s="1">
+        <v>0</v>
+      </c>
+      <c r="F117" s="3"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C118" s="1">
+        <v>0</v>
+      </c>
+      <c r="E118" s="2"/>
+      <c r="F118" s="3"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C119" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C120" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C121" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C122" s="1">
+        <v>0</v>
+      </c>
+      <c r="F122" s="3"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C123" s="1">
+        <v>0</v>
+      </c>
+      <c r="F123" s="3"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C124" s="1">
+        <v>0</v>
+      </c>
+      <c r="F124" s="3"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C125" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C126" s="1">
+        <v>1</v>
+      </c>
+      <c r="E126" s="2"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C127" s="1">
+        <v>1</v>
+      </c>
+      <c r="E127" s="2"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C128" s="1">
+        <v>0</v>
+      </c>
+      <c r="F128" s="3"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C129" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C130" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C131" s="1">
+        <v>0</v>
+      </c>
+      <c r="F131" s="3"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C132" s="1">
+        <v>0</v>
+      </c>
+      <c r="F132" s="3"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C133" s="1">
+        <v>0</v>
+      </c>
+      <c r="F133" s="3"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C134" s="1">
+        <v>0</v>
+      </c>
+      <c r="F134" s="3"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C135" s="1">
+        <v>0</v>
+      </c>
+      <c r="F135" s="3"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C136" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C137" s="1">
+        <v>0</v>
+      </c>
+      <c r="E137" s="2"/>
+      <c r="F137" s="3"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C138" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C139" s="1">
+        <v>0</v>
+      </c>
+      <c r="F139" s="3"/>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C140" s="1">
+        <v>0</v>
+      </c>
+      <c r="F140" s="3"/>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C141" s="1">
+        <v>0</v>
+      </c>
+      <c r="F141" s="3"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C142" s="1">
+        <v>0</v>
+      </c>
+      <c r="F142" s="3"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>59</v>
+      </c>
+      <c r="C143" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>